<commit_message>
Started work on compiling if statements
</commit_message>
<xml_diff>
--- a/Docs/Machine Code for VM.xlsx
+++ b/Docs/Machine Code for VM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming\C++\Typhoon\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{407544BC-E2D9-49A8-A8A9-E97ABD5559B7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC0CD380-7214-49F9-AFA6-4F50957353F5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="190">
   <si>
     <t>BYTECODE</t>
   </si>
@@ -549,9 +549,6 @@
     <t>cgt</t>
   </si>
   <si>
-    <t>Push true to the stack if value 1 is greater then value 2, else push false to the stack</t>
-  </si>
-  <si>
     <t>0x34</t>
   </si>
   <si>
@@ -564,9 +561,6 @@
     <t>clt</t>
   </si>
   <si>
-    <t>Push true to the stack if value 1 is less then value 2, else push false to the stack</t>
-  </si>
-  <si>
     <t>syscall</t>
   </si>
   <si>
@@ -577,6 +571,30 @@
   </si>
   <si>
     <t>0x05</t>
+  </si>
+  <si>
+    <t>0x37</t>
+  </si>
+  <si>
+    <t>0x38</t>
+  </si>
+  <si>
+    <t>cgteq</t>
+  </si>
+  <si>
+    <t>clteq</t>
+  </si>
+  <si>
+    <t>Push true to the stack if value 1 is greater than value 2, else push false to the stack</t>
+  </si>
+  <si>
+    <t>Push true to the stack if value 1 is less than value 2, else push false to the stack</t>
+  </si>
+  <si>
+    <t>Push true to the stack if value 1 is greater than or equal to value 2, else push false to the stack</t>
+  </si>
+  <si>
+    <t>Push true to the stack if value 1 is less than or equal to value 2, else push false to the stack</t>
   </si>
 </sst>
 </file>
@@ -1007,10 +1025,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D56"/>
+  <dimension ref="A1:D58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A56" sqref="A56"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1102,7 +1120,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="B7" t="s">
         <v>22</v>
@@ -1721,38 +1739,60 @@
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B54" t="s">
         <v>173</v>
       </c>
       <c r="D54" t="s">
-        <v>174</v>
+        <v>186</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B55" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D55" t="s">
-        <v>179</v>
+        <v>187</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B56" t="s">
+        <v>184</v>
+      </c>
+      <c r="D56" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>182</v>
+      </c>
+      <c r="B57" t="s">
+        <v>185</v>
+      </c>
+      <c r="D57" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>183</v>
+      </c>
+      <c r="B58" t="s">
+        <v>178</v>
+      </c>
+      <c r="C58" t="s">
+        <v>179</v>
+      </c>
+      <c r="D58" t="s">
         <v>180</v>
-      </c>
-      <c r="C56" t="s">
-        <v>181</v>
-      </c>
-      <c r="D56" t="s">
-        <v>182</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrected if statement compilation
</commit_message>
<xml_diff>
--- a/Docs/Machine Code for VM.xlsx
+++ b/Docs/Machine Code for VM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming\C++\Typhoon\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\C#\Typhoon\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC0CD380-7214-49F9-AFA6-4F50957353F5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C3CFFDD-1E7C-409C-9163-248C97D627B4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -66,78 +66,45 @@
     <t>ldarg.s</t>
   </si>
   <si>
-    <t>&lt;uint8 (num)&gt;</t>
-  </si>
-  <si>
     <t>0x03</t>
   </si>
   <si>
     <t>starg.s</t>
   </si>
   <si>
-    <t>Load argument (num) onto the stack, short form</t>
-  </si>
-  <si>
-    <t>Store value from stack to argument (num), short form</t>
-  </si>
-  <si>
     <t>0x04</t>
   </si>
   <si>
-    <t>&lt;uint16 (num)&gt;</t>
-  </si>
-  <si>
-    <t>Load argument (num) onto the stack</t>
-  </si>
-  <si>
     <t>0x06</t>
   </si>
   <si>
     <t>starg</t>
   </si>
   <si>
-    <t>Store value from stack to argument (num)</t>
-  </si>
-  <si>
     <t>0x07</t>
   </si>
   <si>
     <t>ldarg.l</t>
   </si>
   <si>
-    <t>&lt;uint32 (num)&gt;</t>
-  </si>
-  <si>
-    <t>Load argument (num) onto the stack, long form</t>
-  </si>
-  <si>
     <t>0x08</t>
   </si>
   <si>
     <t>starg.l</t>
   </si>
   <si>
-    <t>Store value from stack to argument (num), long form</t>
-  </si>
-  <si>
     <t>0x09</t>
   </si>
   <si>
     <t>ldloc.s</t>
   </si>
   <si>
-    <t>Load local variable (num) onto the stack</t>
-  </si>
-  <si>
     <t>0x0A</t>
   </si>
   <si>
     <t>stloc.s</t>
   </si>
   <si>
-    <t>Load local variable (num) onto the stack, short form</t>
-  </si>
-  <si>
     <t>0x0B</t>
   </si>
   <si>
@@ -156,9 +123,6 @@
     <t>ldloc.l</t>
   </si>
   <si>
-    <t>Load local variable (num) onto the stack, long form</t>
-  </si>
-  <si>
     <t>stloc.l</t>
   </si>
   <si>
@@ -171,57 +135,30 @@
     <t>load.s</t>
   </si>
   <si>
-    <t>Load global variable (num) onto the stack, short form</t>
-  </si>
-  <si>
     <t>0x10</t>
   </si>
   <si>
     <t>store.s</t>
   </si>
   <si>
-    <t>Store value from stack to local variable (num), long form</t>
-  </si>
-  <si>
-    <t>Store value from stack to local variable (num)</t>
-  </si>
-  <si>
-    <t>Store value from stack to local variable (num), short form</t>
-  </si>
-  <si>
     <t>0x11</t>
   </si>
   <si>
     <t>load</t>
   </si>
   <si>
-    <t>Store value from stack to global variable (num), long form</t>
-  </si>
-  <si>
-    <t>Load global variable (num) onto the stack</t>
-  </si>
-  <si>
     <t>0x12</t>
   </si>
   <si>
     <t>store</t>
   </si>
   <si>
-    <t>Store value from stack to global variable (num)</t>
-  </si>
-  <si>
-    <t>Store value from stack to global variable (num), short form</t>
-  </si>
-  <si>
     <t>0x13</t>
   </si>
   <si>
     <t>load.l</t>
   </si>
   <si>
-    <t>Load global variable (num) onto the stack, long form</t>
-  </si>
-  <si>
     <t>store.l</t>
   </si>
   <si>
@@ -595,6 +532,69 @@
   </si>
   <si>
     <t>Push true to the stack if value 1 is less than or equal to value 2, else push false to the stack</t>
+  </si>
+  <si>
+    <t>&lt;uint8 (index)&gt;</t>
+  </si>
+  <si>
+    <t>Load argument (index) onto the stack, short form</t>
+  </si>
+  <si>
+    <t>Store value from stack to argument (index), short form</t>
+  </si>
+  <si>
+    <t>&lt;uint16 (index)&gt;</t>
+  </si>
+  <si>
+    <t>Load argument (index) onto the stack</t>
+  </si>
+  <si>
+    <t>Store value from stack to argument (index)</t>
+  </si>
+  <si>
+    <t>&lt;uint32 (index)&gt;</t>
+  </si>
+  <si>
+    <t>Load argument (index) onto the stack, long form</t>
+  </si>
+  <si>
+    <t>Store value from stack to argument (index), long form</t>
+  </si>
+  <si>
+    <t>Load local variable (index) onto the stack, short form</t>
+  </si>
+  <si>
+    <t>Store value from stack to local variable (index), short form</t>
+  </si>
+  <si>
+    <t>Load local variable (index) onto the stack</t>
+  </si>
+  <si>
+    <t>Store value from stack to local variable (index)</t>
+  </si>
+  <si>
+    <t>Load local variable (index) onto the stack, long form</t>
+  </si>
+  <si>
+    <t>Store value from stack to local variable (index), long form</t>
+  </si>
+  <si>
+    <t>Load global variable (index) onto the stack, short form</t>
+  </si>
+  <si>
+    <t>Store value from stack to global variable (index), short form</t>
+  </si>
+  <si>
+    <t>Load global variable (index) onto the stack</t>
+  </si>
+  <si>
+    <t>Store value from stack to global variable (index)</t>
+  </si>
+  <si>
+    <t>Load global variable (index) onto the stack, long form</t>
+  </si>
+  <si>
+    <t>Store value from stack to global variable (index), long form</t>
   </si>
 </sst>
 </file>
@@ -1028,19 +1028,19 @@
   <dimension ref="A1:D58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.26953125" customWidth="1"/>
-    <col min="2" max="2" width="15.26953125" customWidth="1"/>
-    <col min="3" max="3" width="34.453125" customWidth="1"/>
-    <col min="4" max="4" width="91.54296875" customWidth="1"/>
-    <col min="5" max="1025" width="11.54296875"/>
+    <col min="1" max="1" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="34.42578125" customWidth="1"/>
+    <col min="4" max="4" width="91.5703125" customWidth="1"/>
+    <col min="5" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1054,7 +1054,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1065,7 +1065,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1076,7 +1076,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1084,715 +1084,715 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
+        <v>169</v>
+      </c>
+      <c r="D4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="B5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
+        <v>169</v>
+      </c>
+      <c r="D5" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>18</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
       <c r="C6" t="s">
+        <v>172</v>
+      </c>
+      <c r="D6" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>160</v>
+      </c>
+      <c r="B7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>172</v>
+      </c>
+      <c r="D7" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
         <v>19</v>
       </c>
-      <c r="D6" t="s">
+      <c r="C8" t="s">
+        <v>175</v>
+      </c>
+      <c r="D8" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" t="s">
+        <v>175</v>
+      </c>
+      <c r="D9" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="B10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" t="s">
+        <v>169</v>
+      </c>
+      <c r="D10" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>169</v>
+      </c>
+      <c r="D11" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
+        <v>172</v>
+      </c>
+      <c r="D12" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="C13" t="s">
+        <v>172</v>
+      </c>
+      <c r="D13" t="s">
         <v>181</v>
       </c>
-      <c r="B7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>21</v>
-      </c>
-      <c r="B8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" t="s">
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" t="s">
+        <v>175</v>
+      </c>
+      <c r="D14" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="B15" t="s">
         <v>32</v>
       </c>
-      <c r="C10" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" t="s">
+      <c r="C15" t="s">
+        <v>175</v>
+      </c>
+      <c r="D15" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>33</v>
+      </c>
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" t="s">
+        <v>169</v>
+      </c>
+      <c r="D16" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" t="s">
+        <v>169</v>
+      </c>
+      <c r="D17" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D11" t="s">
+      <c r="B18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" t="s">
+        <v>172</v>
+      </c>
+      <c r="D18" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+      <c r="B19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" t="s">
+        <v>172</v>
+      </c>
+      <c r="D19" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>40</v>
+      </c>
+      <c r="B20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" t="s">
+        <v>175</v>
+      </c>
+      <c r="D20" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>42</v>
+      </c>
+      <c r="B21" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" t="s">
+        <v>175</v>
+      </c>
+      <c r="D21" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" t="s">
+        <v>47</v>
+      </c>
+      <c r="D22" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" t="s">
+        <v>52</v>
+      </c>
+      <c r="D23" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>49</v>
+      </c>
+      <c r="B24" t="s">
+        <v>54</v>
+      </c>
+      <c r="C24" t="s">
+        <v>55</v>
+      </c>
+      <c r="D24" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" t="s">
-        <v>38</v>
-      </c>
-      <c r="C12" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>37</v>
-      </c>
-      <c r="B13" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" t="s">
-        <v>19</v>
-      </c>
-      <c r="D13" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" t="s">
-        <v>42</v>
-      </c>
-      <c r="C14" t="s">
-        <v>26</v>
-      </c>
-      <c r="D14" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>41</v>
-      </c>
-      <c r="B15" t="s">
-        <v>44</v>
-      </c>
-      <c r="C15" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>45</v>
-      </c>
-      <c r="B16" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" t="s">
-        <v>13</v>
-      </c>
-      <c r="D16" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>46</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="B25" t="s">
         <v>50</v>
       </c>
-      <c r="C17" t="s">
-        <v>13</v>
-      </c>
-      <c r="D17" t="s">
+      <c r="C25" t="s">
+        <v>57</v>
+      </c>
+      <c r="D25" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>49</v>
-      </c>
-      <c r="B18" t="s">
-        <v>55</v>
-      </c>
-      <c r="C18" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>54</v>
-      </c>
-      <c r="B19" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>56</v>
+      </c>
+      <c r="B26" t="s">
         <v>59</v>
       </c>
-      <c r="C19" t="s">
-        <v>19</v>
-      </c>
-      <c r="D19" t="s">
+      <c r="C26" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="D26" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
         <v>58</v>
       </c>
-      <c r="B20" t="s">
-        <v>63</v>
-      </c>
-      <c r="C20" t="s">
-        <v>26</v>
-      </c>
-      <c r="D20" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>62</v>
-      </c>
-      <c r="B21" t="s">
+      <c r="B27" t="s">
+        <v>67</v>
+      </c>
+      <c r="C27" t="s">
+        <v>69</v>
+      </c>
+      <c r="D27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
         <v>65</v>
       </c>
-      <c r="C21" t="s">
-        <v>26</v>
-      </c>
-      <c r="D21" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="B28" t="s">
+        <v>68</v>
+      </c>
+      <c r="C28" t="s">
+        <v>70</v>
+      </c>
+      <c r="D28" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
         <v>66</v>
       </c>
-      <c r="B22" t="s">
-        <v>68</v>
-      </c>
-      <c r="D22" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>67</v>
-      </c>
-      <c r="B23" t="s">
-        <v>72</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="B29" t="s">
+        <v>74</v>
+      </c>
+      <c r="C29" t="s">
+        <v>75</v>
+      </c>
+      <c r="D29" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>73</v>
       </c>
-      <c r="D23" t="s">
+      <c r="B30" t="s">
+        <v>78</v>
+      </c>
+      <c r="C30" t="s">
+        <v>79</v>
+      </c>
+      <c r="D30" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" t="s">
+        <v>82</v>
+      </c>
+      <c r="C31" t="s">
+        <v>83</v>
+      </c>
+      <c r="D31" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>70</v>
-      </c>
-      <c r="B24" t="s">
-        <v>75</v>
-      </c>
-      <c r="C24" t="s">
-        <v>76</v>
-      </c>
-      <c r="D24" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>74</v>
-      </c>
-      <c r="B25" t="s">
-        <v>71</v>
-      </c>
-      <c r="C25" t="s">
-        <v>78</v>
-      </c>
-      <c r="D25" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>77</v>
-      </c>
-      <c r="B26" t="s">
-        <v>80</v>
-      </c>
-      <c r="C26" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
         <v>81</v>
       </c>
-      <c r="D26" t="s">
+      <c r="B32" t="s">
+        <v>86</v>
+      </c>
+      <c r="D32" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>79</v>
-      </c>
-      <c r="B27" t="s">
+      <c r="B33" t="s">
+        <v>89</v>
+      </c>
+      <c r="D33" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
         <v>88</v>
       </c>
-      <c r="C27" t="s">
-        <v>90</v>
-      </c>
-      <c r="D27" t="s">
+      <c r="B34" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>86</v>
-      </c>
-      <c r="B28" t="s">
-        <v>89</v>
-      </c>
-      <c r="C28" t="s">
+      <c r="C34" t="s">
+        <v>93</v>
+      </c>
+      <c r="D34" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
         <v>91</v>
       </c>
-      <c r="D28" t="s">
+      <c r="B35" t="s">
+        <v>95</v>
+      </c>
+      <c r="C35" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>87</v>
-      </c>
-      <c r="B29" t="s">
-        <v>95</v>
-      </c>
-      <c r="C29" t="s">
+      <c r="D35" t="s">
         <v>96</v>
       </c>
-      <c r="D29" t="s">
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
         <v>97</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+      <c r="B36" t="s">
+        <v>99</v>
+      </c>
+      <c r="C36" t="s">
+        <v>93</v>
+      </c>
+      <c r="D36" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>98</v>
+      </c>
+      <c r="B37" t="s">
+        <v>104</v>
+      </c>
+      <c r="C37" t="s">
+        <v>107</v>
+      </c>
+      <c r="D37" t="s">
         <v>94</v>
       </c>
-      <c r="B30" t="s">
-        <v>99</v>
-      </c>
-      <c r="C30" t="s">
-        <v>100</v>
-      </c>
-      <c r="D30" t="s">
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>98</v>
-      </c>
-      <c r="B31" t="s">
+      <c r="B38" t="s">
+        <v>105</v>
+      </c>
+      <c r="C38" t="s">
+        <v>107</v>
+      </c>
+      <c r="D38" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>102</v>
+      </c>
+      <c r="B39" t="s">
+        <v>106</v>
+      </c>
+      <c r="C39" t="s">
+        <v>107</v>
+      </c>
+      <c r="D39" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
         <v>103</v>
       </c>
-      <c r="C31" t="s">
-        <v>104</v>
-      </c>
-      <c r="D31" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>102</v>
-      </c>
-      <c r="B32" t="s">
-        <v>107</v>
-      </c>
-      <c r="D32" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>106</v>
-      </c>
-      <c r="B33" t="s">
+      <c r="B40" t="s">
         <v>110</v>
       </c>
-      <c r="D33" t="s">
+      <c r="C40" t="s">
+        <v>116</v>
+      </c>
+      <c r="D40" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>113</v>
+      </c>
+      <c r="B41" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>109</v>
-      </c>
-      <c r="B34" t="s">
-        <v>113</v>
-      </c>
-      <c r="C34" t="s">
+      <c r="C41" t="s">
+        <v>116</v>
+      </c>
+      <c r="D41" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
         <v>114</v>
       </c>
-      <c r="D34" t="s">
+      <c r="B42" t="s">
+        <v>112</v>
+      </c>
+      <c r="C42" t="s">
+        <v>116</v>
+      </c>
+      <c r="D42" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>112</v>
-      </c>
-      <c r="B35" t="s">
+      <c r="B43" t="s">
+        <v>130</v>
+      </c>
+      <c r="D43" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>122</v>
+      </c>
+      <c r="B44" t="s">
+        <v>131</v>
+      </c>
+      <c r="D44" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>123</v>
+      </c>
+      <c r="B45" t="s">
+        <v>132</v>
+      </c>
+      <c r="C45" t="s">
         <v>116</v>
       </c>
-      <c r="C35" t="s">
-        <v>114</v>
-      </c>
-      <c r="D35" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>118</v>
-      </c>
-      <c r="B36" t="s">
+      <c r="D45" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>126</v>
+      </c>
+      <c r="B46" t="s">
+        <v>133</v>
+      </c>
+      <c r="D46" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>127</v>
+      </c>
+      <c r="B47" t="s">
         <v>120</v>
       </c>
-      <c r="C36" t="s">
-        <v>114</v>
-      </c>
-      <c r="D36" t="s">
+      <c r="D47" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>119</v>
-      </c>
-      <c r="B37" t="s">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>128</v>
+      </c>
+      <c r="B48" t="s">
+        <v>124</v>
+      </c>
+      <c r="D48" t="s">
         <v>125</v>
       </c>
-      <c r="C37" t="s">
-        <v>128</v>
-      </c>
-      <c r="D37" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>122</v>
-      </c>
-      <c r="B38" t="s">
-        <v>126</v>
-      </c>
-      <c r="C38" t="s">
-        <v>128</v>
-      </c>
-      <c r="D38" t="s">
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>123</v>
-      </c>
-      <c r="B39" t="s">
-        <v>127</v>
-      </c>
-      <c r="C39" t="s">
-        <v>128</v>
-      </c>
-      <c r="D39" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>124</v>
-      </c>
-      <c r="B40" t="s">
-        <v>131</v>
-      </c>
-      <c r="C40" t="s">
-        <v>137</v>
-      </c>
-      <c r="D40" t="s">
+      <c r="B49" t="s">
+        <v>139</v>
+      </c>
+      <c r="D49" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>134</v>
-      </c>
-      <c r="B41" t="s">
-        <v>132</v>
-      </c>
-      <c r="C41" t="s">
-        <v>137</v>
-      </c>
-      <c r="D41" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>135</v>
-      </c>
-      <c r="B42" t="s">
-        <v>133</v>
-      </c>
-      <c r="C42" t="s">
-        <v>137</v>
-      </c>
-      <c r="D42" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>136</v>
-      </c>
-      <c r="B43" t="s">
+      <c r="B50" t="s">
+        <v>142</v>
+      </c>
+      <c r="D50" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51" t="s">
+        <v>141</v>
+      </c>
+      <c r="B51" t="s">
+        <v>145</v>
+      </c>
+      <c r="D51" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52" t="s">
+        <v>144</v>
+      </c>
+      <c r="B52" t="s">
+        <v>148</v>
+      </c>
+      <c r="D52" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
+        <v>147</v>
+      </c>
+      <c r="B53" t="s">
+        <v>150</v>
+      </c>
+      <c r="D53" t="s">
         <v>151</v>
       </c>
-      <c r="D43" t="s">
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
+        <v>153</v>
+      </c>
+      <c r="B54" t="s">
+        <v>152</v>
+      </c>
+      <c r="D54" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55" t="s">
+        <v>154</v>
+      </c>
+      <c r="B55" t="s">
+        <v>156</v>
+      </c>
+      <c r="D55" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>143</v>
-      </c>
-      <c r="B44" t="s">
-        <v>152</v>
-      </c>
-      <c r="D44" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>144</v>
-      </c>
-      <c r="B45" t="s">
-        <v>153</v>
-      </c>
-      <c r="C45" t="s">
-        <v>137</v>
-      </c>
-      <c r="D45" t="s">
+      <c r="B56" t="s">
+        <v>163</v>
+      </c>
+      <c r="D56" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57" t="s">
+        <v>161</v>
+      </c>
+      <c r="B57" t="s">
+        <v>164</v>
+      </c>
+      <c r="D57" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>162</v>
+      </c>
+      <c r="B58" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>147</v>
-      </c>
-      <c r="B46" t="s">
-        <v>154</v>
-      </c>
-      <c r="D46" t="s">
+      <c r="C58" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>148</v>
-      </c>
-      <c r="B47" t="s">
-        <v>141</v>
-      </c>
-      <c r="D47" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>149</v>
-      </c>
-      <c r="B48" t="s">
-        <v>145</v>
-      </c>
-      <c r="D48" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>150</v>
-      </c>
-      <c r="B49" t="s">
-        <v>160</v>
-      </c>
-      <c r="D49" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
+      <c r="D58" t="s">
         <v>159</v>
-      </c>
-      <c r="B50" t="s">
-        <v>163</v>
-      </c>
-      <c r="D50" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>162</v>
-      </c>
-      <c r="B51" t="s">
-        <v>166</v>
-      </c>
-      <c r="D51" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>165</v>
-      </c>
-      <c r="B52" t="s">
-        <v>169</v>
-      </c>
-      <c r="D52" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>168</v>
-      </c>
-      <c r="B53" t="s">
-        <v>171</v>
-      </c>
-      <c r="D53" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>174</v>
-      </c>
-      <c r="B54" t="s">
-        <v>173</v>
-      </c>
-      <c r="D54" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>175</v>
-      </c>
-      <c r="B55" t="s">
-        <v>177</v>
-      </c>
-      <c r="D55" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>176</v>
-      </c>
-      <c r="B56" t="s">
-        <v>184</v>
-      </c>
-      <c r="D56" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>182</v>
-      </c>
-      <c r="B57" t="s">
-        <v>185</v>
-      </c>
-      <c r="D57" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>183</v>
-      </c>
-      <c r="B58" t="s">
-        <v>178</v>
-      </c>
-      <c r="C58" t="s">
-        <v>179</v>
-      </c>
-      <c r="D58" t="s">
-        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Basics of arrays + fixes
</commit_message>
<xml_diff>
--- a/Docs/Machine Code for VM.xlsx
+++ b/Docs/Machine Code for VM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming\C#\Typhoon\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming\C++\Typhoon\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C3CFFDD-1E7C-409C-9163-248C97D627B4}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB8CAB9-06DC-41EA-8EAE-BF999D129F66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="199">
   <si>
     <t>BYTECODE</t>
   </si>
@@ -595,6 +595,33 @@
   </si>
   <si>
     <t>Store value from stack to global variable (index), long form</t>
+  </si>
+  <si>
+    <t>0x39</t>
+  </si>
+  <si>
+    <t>newarray</t>
+  </si>
+  <si>
+    <t>Push a new array object to the stack</t>
+  </si>
+  <si>
+    <t>0x3A</t>
+  </si>
+  <si>
+    <t>aload</t>
+  </si>
+  <si>
+    <t>Load an object from the array ontop of the stack to the stack</t>
+  </si>
+  <si>
+    <t>0x3B</t>
+  </si>
+  <si>
+    <t>astore</t>
+  </si>
+  <si>
+    <t>Store an object ontop of the stack to and array now ontop of the stack</t>
   </si>
 </sst>
 </file>
@@ -1025,22 +1052,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D58"/>
+  <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="3" max="3" width="34.42578125" customWidth="1"/>
-    <col min="4" max="4" width="91.5703125" customWidth="1"/>
-    <col min="5" max="1025" width="11.5703125"/>
+    <col min="1" max="1" width="14.26953125" customWidth="1"/>
+    <col min="2" max="2" width="15.26953125" customWidth="1"/>
+    <col min="3" max="3" width="34.453125" customWidth="1"/>
+    <col min="4" max="4" width="91.54296875" customWidth="1"/>
+    <col min="5" max="1025" width="11.54296875"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1054,7 +1081,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1065,7 +1092,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1076,7 +1103,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -1090,7 +1117,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1104,7 +1131,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -1118,7 +1145,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>160</v>
       </c>
@@ -1132,7 +1159,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -1146,7 +1173,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -1160,7 +1187,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>20</v>
       </c>
@@ -1174,7 +1201,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>22</v>
       </c>
@@ -1188,7 +1215,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1202,7 +1229,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -1216,7 +1243,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>28</v>
       </c>
@@ -1230,7 +1257,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>30</v>
       </c>
@@ -1244,7 +1271,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -1258,7 +1285,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>34</v>
       </c>
@@ -1272,7 +1299,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>36</v>
       </c>
@@ -1286,7 +1313,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -1300,7 +1327,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>40</v>
       </c>
@@ -1314,7 +1341,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>42</v>
       </c>
@@ -1328,7 +1355,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>45</v>
       </c>
@@ -1339,7 +1366,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>46</v>
       </c>
@@ -1353,7 +1380,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>49</v>
       </c>
@@ -1367,7 +1394,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>53</v>
       </c>
@@ -1381,7 +1408,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>56</v>
       </c>
@@ -1395,7 +1422,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>58</v>
       </c>
@@ -1409,7 +1436,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>65</v>
       </c>
@@ -1423,7 +1450,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>66</v>
       </c>
@@ -1437,7 +1464,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>73</v>
       </c>
@@ -1451,7 +1478,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>77</v>
       </c>
@@ -1465,7 +1492,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>81</v>
       </c>
@@ -1476,7 +1503,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>85</v>
       </c>
@@ -1487,7 +1514,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>88</v>
       </c>
@@ -1501,7 +1528,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>91</v>
       </c>
@@ -1515,7 +1542,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>97</v>
       </c>
@@ -1529,7 +1556,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>98</v>
       </c>
@@ -1543,7 +1570,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>101</v>
       </c>
@@ -1557,7 +1584,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>102</v>
       </c>
@@ -1571,7 +1598,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>103</v>
       </c>
@@ -1585,7 +1612,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>113</v>
       </c>
@@ -1599,7 +1626,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>114</v>
       </c>
@@ -1613,7 +1640,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>115</v>
       </c>
@@ -1624,7 +1651,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>122</v>
       </c>
@@ -1635,7 +1662,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>123</v>
       </c>
@@ -1649,7 +1676,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>126</v>
       </c>
@@ -1660,7 +1687,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>127</v>
       </c>
@@ -1671,7 +1698,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>128</v>
       </c>
@@ -1682,7 +1709,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>129</v>
       </c>
@@ -1693,7 +1720,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>138</v>
       </c>
@@ -1704,7 +1731,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>141</v>
       </c>
@@ -1715,7 +1742,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>144</v>
       </c>
@@ -1726,7 +1753,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>147</v>
       </c>
@@ -1737,7 +1764,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>153</v>
       </c>
@@ -1748,7 +1775,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>154</v>
       </c>
@@ -1759,7 +1786,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>155</v>
       </c>
@@ -1770,7 +1797,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>161</v>
       </c>
@@ -1781,7 +1808,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>162</v>
       </c>
@@ -1793,6 +1820,39 @@
       </c>
       <c r="D58" t="s">
         <v>159</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>190</v>
+      </c>
+      <c r="B59" t="s">
+        <v>191</v>
+      </c>
+      <c r="D59" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>193</v>
+      </c>
+      <c r="B60" t="s">
+        <v>194</v>
+      </c>
+      <c r="D60" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>196</v>
+      </c>
+      <c r="B61" t="s">
+        <v>197</v>
+      </c>
+      <c r="D61" t="s">
+        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Get objects in an array and multi-dimensional arrays
</commit_message>
<xml_diff>
--- a/Docs/Machine Code for VM.xlsx
+++ b/Docs/Machine Code for VM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Programming\C++\Typhoon\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB8CAB9-06DC-41EA-8EAE-BF999D129F66}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B43ABE96-93D7-4CD9-B3E6-FC6BEA48F228}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="57480" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -612,9 +612,6 @@
     <t>aload</t>
   </si>
   <si>
-    <t>Load an object from the array ontop of the stack to the stack</t>
-  </si>
-  <si>
     <t>0x3B</t>
   </si>
   <si>
@@ -622,6 +619,9 @@
   </si>
   <si>
     <t>Store an object ontop of the stack to and array now ontop of the stack</t>
+  </si>
+  <si>
+    <t>Load an object from the array at the index specified from the top of the stack to the stack</t>
   </si>
 </sst>
 </file>
@@ -1054,8 +1054,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D62" sqref="D62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1841,18 +1841,18 @@
         <v>194</v>
       </c>
       <c r="D60" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>195</v>
+      </c>
+      <c r="B61" t="s">
         <v>196</v>
       </c>
-      <c r="B61" t="s">
+      <c r="D61" t="s">
         <v>197</v>
-      </c>
-      <c r="D61" t="s">
-        <v>198</v>
       </c>
     </row>
   </sheetData>

</xml_diff>